<commit_message>
my backup files dated 12.05.2020
</commit_message>
<xml_diff>
--- a/Financial statements.xlsx
+++ b/Financial statements.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -22,18 +21,12 @@
     <t>Sales - Net</t>
   </si>
   <si>
-    <t>Cheety</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total </t>
   </si>
   <si>
     <t>Pizza Velly</t>
   </si>
   <si>
-    <t>Food Panda</t>
-  </si>
-  <si>
     <t>Trattoria</t>
   </si>
   <si>
@@ -104,6 +97,12 @@
   </si>
   <si>
     <t>Maida consumed</t>
+  </si>
+  <si>
+    <t>Cheety - Sales</t>
+  </si>
+  <si>
+    <t>Food Panda - Sales</t>
   </si>
 </sst>
 </file>
@@ -113,9 +112,9 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;_-* #,##0.00\-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;_-* #,##0\-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,16 +218,66 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -288,12 +337,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -311,12 +375,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -324,19 +384,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -357,22 +404,106 @@
     <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -382,6 +513,63 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1638300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>457200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Right Brace 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2105025" y="5410200"/>
+          <a:ext cx="314325" cy="409575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -672,17 +860,17 @@
   <dimension ref="B1:O89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:M1"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
     <col min="4" max="4" width="2.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -695,96 +883,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="23.25">
-      <c r="B1" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
+      <c r="B1" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
     </row>
     <row r="2" spans="2:15" ht="23.25">
-      <c r="B2" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
+      <c r="B2" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
     </row>
     <row r="3" spans="2:15" ht="23.25">
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
     </row>
     <row r="4" spans="2:15" ht="18.75">
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="29" t="s">
+      <c r="H4" s="37"/>
+      <c r="I4" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="29" t="s">
+      <c r="J4" s="37"/>
+      <c r="K4" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="38"/>
+      <c r="M4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="30"/>
-      <c r="K4" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="31"/>
-      <c r="M4" s="29" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="5" spans="2:15" ht="21">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="16">
         <v>1</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27">
+      <c r="F5" s="17"/>
+      <c r="G5" s="58">
         <f>G10/E10</f>
         <v>0.74320389428526978</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="27">
+      <c r="H5" s="19"/>
+      <c r="I5" s="56">
         <f>I10/E10</f>
         <v>3.5071906466025031E-2</v>
       </c>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27">
+      <c r="J5" s="18"/>
+      <c r="K5" s="58">
         <f>K10/E10</f>
         <v>7.2354353286358891E-2</v>
       </c>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27">
+      <c r="L5" s="18"/>
+      <c r="M5" s="56">
         <f>M10/E10</f>
         <v>0.14936984596234634</v>
       </c>
@@ -792,116 +980,125 @@
     </row>
     <row r="6" spans="2:15" ht="21" customHeight="1">
       <c r="C6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="9">
+        <v>27</v>
+      </c>
+      <c r="E6" s="40">
         <v>1346370</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="9">
+      <c r="F6" s="25">
+        <f>E6/E$10</f>
+        <v>0.74816621840894437</v>
+      </c>
+      <c r="G6" s="29">
         <v>1337440</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="9">
+      <c r="H6" s="30"/>
+      <c r="I6" s="29">
         <v>425</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="9">
+      <c r="J6" s="30"/>
+      <c r="K6" s="29">
         <v>8505</v>
       </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="9">
+      <c r="L6" s="30"/>
+      <c r="M6" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="21" customHeight="1">
       <c r="C7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="11">
+        <v>28</v>
+      </c>
+      <c r="E7" s="41">
         <v>184390</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11">
+      <c r="F7" s="25">
+        <f>E7/E$10</f>
+        <v>0.10246393562870924</v>
+      </c>
+      <c r="G7" s="31">
         <v>0</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="11">
+      <c r="H7" s="30"/>
+      <c r="I7" s="31">
         <v>62689</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="11">
+      <c r="J7" s="30"/>
+      <c r="K7" s="31">
         <v>121701</v>
       </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="11">
+      <c r="L7" s="30"/>
+      <c r="M7" s="31">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="21" customHeight="1">
       <c r="C8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="12">
+        <v>25</v>
+      </c>
+      <c r="E8" s="42">
         <v>268800</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="12">
+      <c r="F8" s="25">
+        <f>E8/E$10</f>
+        <v>0.14936984596234634</v>
+      </c>
+      <c r="G8" s="32">
         <v>0</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="12">
+      <c r="H8" s="30"/>
+      <c r="I8" s="32">
         <v>0</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="12">
+      <c r="J8" s="30"/>
+      <c r="K8" s="32">
         <v>0</v>
       </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="12">
+      <c r="L8" s="30"/>
+      <c r="M8" s="32">
         <v>268800</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="4.5" customHeight="1">
       <c r="C9" s="7"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="13"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="33"/>
     </row>
     <row r="10" spans="2:15" ht="19.5">
-      <c r="C10" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="14">
+      <c r="C10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="43">
         <f>SUM(E6:E8)</f>
         <v>1799560</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="45">
         <f>E10/E10</f>
         <v>1</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="34">
         <f>SUM(G6:G8)</f>
         <v>1337440</v>
       </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="14">
+      <c r="H10" s="35"/>
+      <c r="I10" s="34">
         <f>SUM(I6:I8)</f>
         <v>63114</v>
       </c>
-      <c r="J10" s="15"/>
-      <c r="K10" s="14">
+      <c r="J10" s="35"/>
+      <c r="K10" s="34">
         <f>SUM(K6:K8)</f>
         <v>130206</v>
       </c>
-      <c r="L10" s="16"/>
-      <c r="M10" s="14">
+      <c r="L10" s="36"/>
+      <c r="M10" s="34">
         <f>SUM(M6:M8)</f>
         <v>268800</v>
       </c>
@@ -909,175 +1106,190 @@
     </row>
     <row r="11" spans="2:15" ht="17.25">
       <c r="C11" s="7"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="17"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="13"/>
       <c r="N11" s="5"/>
     </row>
     <row r="12" spans="2:15" ht="21">
-      <c r="B12" s="23" t="s">
-        <v>9</v>
+      <c r="B12" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="17"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="13"/>
       <c r="N12" s="5"/>
     </row>
-    <row r="13" spans="2:15" ht="17.25">
+    <row r="13" spans="2:15" ht="18.75">
       <c r="C13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="9">
+        <v>8</v>
+      </c>
+      <c r="E13" s="40">
         <v>201281</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="9">
+      <c r="F13" s="25">
+        <f>E13/E$10</f>
+        <v>0.11185011891795772</v>
+      </c>
+      <c r="G13" s="29">
         <f>E13*0.7432-10</f>
         <v>149582.0392</v>
       </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="9">
+      <c r="H13" s="36"/>
+      <c r="I13" s="29">
         <f>E13*0.0351</f>
         <v>7064.9630999999999</v>
       </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="9">
+      <c r="J13" s="36"/>
+      <c r="K13" s="29">
         <f>E13*0.0724</f>
         <v>14572.744400000001</v>
       </c>
-      <c r="L13" s="16"/>
-      <c r="M13" s="9">
+      <c r="L13" s="36"/>
+      <c r="M13" s="29">
         <f>E13*0.1494-10</f>
         <v>30061.381400000002</v>
       </c>
       <c r="N13" s="5"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="14" spans="2:15" ht="17.25">
+    <row r="14" spans="2:15" ht="18.75">
       <c r="C14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="11">
+        <v>9</v>
+      </c>
+      <c r="E14" s="41">
         <v>351000</v>
       </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="11">
+      <c r="F14" s="25">
+        <f>E14/E$10</f>
+        <v>0.19504767832136743</v>
+      </c>
+      <c r="G14" s="31">
         <f>E14*0.7432-20</f>
         <v>260843.19999999998</v>
       </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="11">
+      <c r="H14" s="36"/>
+      <c r="I14" s="31">
         <f>E14*0.0351</f>
         <v>12320.1</v>
       </c>
-      <c r="J14" s="16"/>
-      <c r="K14" s="11">
+      <c r="J14" s="36"/>
+      <c r="K14" s="31">
         <f>E14*0.0724</f>
         <v>25412.400000000001</v>
       </c>
-      <c r="L14" s="16"/>
-      <c r="M14" s="11">
+      <c r="L14" s="36"/>
+      <c r="M14" s="31">
         <f>E14*0.1494-14</f>
         <v>52425.4</v>
       </c>
       <c r="N14" s="5"/>
     </row>
-    <row r="15" spans="2:15" ht="17.25">
+    <row r="15" spans="2:15" ht="18.75">
       <c r="C15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="11">
+        <v>10</v>
+      </c>
+      <c r="E15" s="41">
         <v>26200</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="11">
+      <c r="F15" s="25">
+        <f>E15/E$10</f>
+        <v>1.4559114450198937E-2</v>
+      </c>
+      <c r="G15" s="31">
         <f>E15*0.7432-3</f>
         <v>19468.84</v>
       </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="11">
+      <c r="H15" s="36"/>
+      <c r="I15" s="31">
         <f>E15*0.0351</f>
         <v>919.62</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="11">
+      <c r="J15" s="36"/>
+      <c r="K15" s="31">
         <f>E15*0.0724</f>
         <v>1896.88</v>
       </c>
-      <c r="L15" s="16"/>
-      <c r="M15" s="11">
+      <c r="L15" s="36"/>
+      <c r="M15" s="31">
         <f>E15*0.1494</f>
         <v>3914.28</v>
       </c>
       <c r="N15" s="5"/>
     </row>
-    <row r="16" spans="2:15" ht="17.25">
+    <row r="16" spans="2:15" ht="18.75">
       <c r="C16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="11">
+        <v>11</v>
+      </c>
+      <c r="E16" s="41">
         <f>10*3100</f>
         <v>31000</v>
       </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="11">
+      <c r="F16" s="25">
+        <f>E16/E$10</f>
+        <v>1.7226433128097979E-2</v>
+      </c>
+      <c r="G16" s="31">
         <f>E16*0.7432-3</f>
         <v>23036.2</v>
       </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="11">
+      <c r="H16" s="36"/>
+      <c r="I16" s="31">
         <f>E16*0.0351</f>
         <v>1088.0999999999999</v>
       </c>
-      <c r="J16" s="16"/>
-      <c r="K16" s="11">
+      <c r="J16" s="36"/>
+      <c r="K16" s="31">
         <f>E16*0.0724</f>
         <v>2244.4</v>
       </c>
-      <c r="L16" s="16"/>
-      <c r="M16" s="11">
+      <c r="L16" s="36"/>
+      <c r="M16" s="31">
         <f>E16*0.1494</f>
         <v>4631.4000000000005</v>
       </c>
       <c r="N16" s="5"/>
     </row>
-    <row r="17" spans="2:15" ht="17.25">
+    <row r="17" spans="2:15" ht="18.75">
       <c r="C17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="12">
+        <v>26</v>
+      </c>
+      <c r="E17" s="42">
         <v>36000</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="12">
+      <c r="F17" s="25">
+        <f>E17/E$10</f>
+        <v>2.0004890084242815E-2</v>
+      </c>
+      <c r="G17" s="32">
         <f>E17*0.7432-4</f>
         <v>26751.200000000001</v>
       </c>
-      <c r="H17" s="16"/>
-      <c r="I17" s="12">
+      <c r="H17" s="36"/>
+      <c r="I17" s="32">
         <f>E17*0.0351</f>
         <v>1263.5999999999999</v>
       </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="12">
+      <c r="J17" s="36"/>
+      <c r="K17" s="32">
         <f>E17*0.0724</f>
         <v>2606.4</v>
       </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="12">
+      <c r="L17" s="36"/>
+      <c r="M17" s="32">
         <f>E17*0.1494</f>
         <v>5378.4000000000005</v>
       </c>
@@ -1085,278 +1297,293 @@
     </row>
     <row r="18" spans="2:15" ht="3.75" customHeight="1">
       <c r="C18" s="7"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="17"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="39"/>
       <c r="N18" s="5"/>
     </row>
     <row r="19" spans="2:15" ht="19.5">
-      <c r="C19" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="14">
+      <c r="C19" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="47">
         <f>SUM(E13:E17)</f>
         <v>645481</v>
       </c>
-      <c r="F19" s="36">
+      <c r="F19" s="46">
         <f>E19/E10</f>
         <v>0.35868823490186491</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="34">
         <f>SUM(G13:G16)</f>
         <v>452930.27919999999</v>
       </c>
-      <c r="H19" s="15"/>
-      <c r="I19" s="14">
+      <c r="H19" s="35"/>
+      <c r="I19" s="34">
         <f>SUM(I13:I17)</f>
         <v>22656.383099999995</v>
       </c>
-      <c r="J19" s="15"/>
-      <c r="K19" s="14">
+      <c r="J19" s="35"/>
+      <c r="K19" s="34">
         <f>SUM(K13:K17)</f>
         <v>46732.824400000005</v>
       </c>
-      <c r="L19" s="15"/>
-      <c r="M19" s="14">
+      <c r="L19" s="35"/>
+      <c r="M19" s="34">
         <f>SUM(M13:M16)</f>
         <v>91032.4614</v>
       </c>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="2:15" ht="17.25">
+    <row r="20" spans="2:15" ht="12" customHeight="1">
       <c r="C20" s="7"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="17"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="39"/>
       <c r="N20" s="5"/>
     </row>
     <row r="21" spans="2:15" ht="21">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="2:15" ht="18.75">
+      <c r="C22" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="5"/>
-    </row>
-    <row r="22" spans="2:15" ht="17.25">
-      <c r="C22" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="9">
+      <c r="E22" s="40">
         <f>E6*0.21</f>
         <v>282737.7</v>
       </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="9">
+      <c r="F22" s="25"/>
+      <c r="G22" s="29">
         <f>G6/1346370*E22</f>
         <v>280862.40000000002</v>
       </c>
-      <c r="H22" s="16"/>
-      <c r="I22" s="9">
+      <c r="H22" s="36"/>
+      <c r="I22" s="29">
         <f>I6/1346370*E22</f>
         <v>89.25</v>
       </c>
-      <c r="J22" s="16"/>
-      <c r="K22" s="9">
+      <c r="J22" s="36"/>
+      <c r="K22" s="29">
         <f>K6/1346370*E22</f>
         <v>1786.0500000000002</v>
       </c>
-      <c r="L22" s="16"/>
-      <c r="M22" s="9">
+      <c r="L22" s="36"/>
+      <c r="M22" s="29">
         <v>0</v>
       </c>
       <c r="N22" s="5"/>
-      <c r="O22" s="35"/>
-    </row>
-    <row r="23" spans="2:15" ht="17.25">
+      <c r="O22" s="23"/>
+    </row>
+    <row r="23" spans="2:15" ht="18.75">
       <c r="C23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="11">
+        <v>15</v>
+      </c>
+      <c r="E23" s="41">
         <f>E7*0.25</f>
         <v>46097.5</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="11">
+      <c r="F23" s="25"/>
+      <c r="G23" s="31">
         <f>G7/184390*E23</f>
         <v>0</v>
       </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="11">
+      <c r="H23" s="36"/>
+      <c r="I23" s="31">
         <f>I7/184390*E23</f>
         <v>15672.249999999998</v>
       </c>
-      <c r="J23" s="16"/>
-      <c r="K23" s="11">
+      <c r="J23" s="36"/>
+      <c r="K23" s="31">
         <f>K7/184390*E23</f>
         <v>30425.25</v>
       </c>
-      <c r="L23" s="16"/>
-      <c r="M23" s="11">
+      <c r="L23" s="36"/>
+      <c r="M23" s="31">
         <v>0</v>
       </c>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" spans="2:15" ht="34.5" customHeight="1">
+    <row r="24" spans="2:15" ht="38.25" customHeight="1">
       <c r="C24" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="18">
+        <v>17</v>
+      </c>
+      <c r="E24" s="41">
         <v>142209</v>
       </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="18">
+      <c r="F24" s="25">
+        <f>E24/E$10</f>
+        <v>7.902431705528018E-2</v>
+      </c>
+      <c r="G24" s="31">
         <f>E24*0.7432-4</f>
         <v>105685.7288</v>
       </c>
-      <c r="H24" s="20"/>
-      <c r="I24" s="18">
+      <c r="H24" s="36"/>
+      <c r="I24" s="31">
         <f>E24*0.0351</f>
         <v>4991.5358999999999</v>
       </c>
-      <c r="J24" s="20"/>
-      <c r="K24" s="18">
+      <c r="J24" s="36"/>
+      <c r="K24" s="31">
         <f>E24*0.0724</f>
         <v>10295.931600000002</v>
       </c>
-      <c r="L24" s="20"/>
-      <c r="M24" s="18">
+      <c r="L24" s="36"/>
+      <c r="M24" s="31">
         <f>E24*0.1494-10</f>
         <v>21236.024600000001</v>
       </c>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" spans="2:15" ht="17.25">
+    <row r="25" spans="2:15" ht="18.75">
       <c r="C25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="41">
+        <v>30000</v>
+      </c>
+      <c r="F25" s="25">
+        <f>E25/E$10</f>
+        <v>1.6670741736869013E-2</v>
+      </c>
+      <c r="G25" s="31">
+        <f>E25*0.7432-2</f>
+        <v>22294</v>
+      </c>
+      <c r="H25" s="36"/>
+      <c r="I25" s="31">
+        <f>E25*0.0351</f>
+        <v>1053</v>
+      </c>
+      <c r="J25" s="36"/>
+      <c r="K25" s="31">
+        <f>E25*0.0724</f>
+        <v>2172</v>
+      </c>
+      <c r="L25" s="36"/>
+      <c r="M25" s="31">
+        <f>E25*0.1494</f>
+        <v>4482</v>
+      </c>
+      <c r="N25" s="5"/>
+    </row>
+    <row r="26" spans="2:15" ht="18.75">
+      <c r="C26" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="11">
-        <v>20000</v>
-      </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="18">
-        <f>E25*0.7432-2</f>
-        <v>14862</v>
-      </c>
-      <c r="H25" s="20"/>
-      <c r="I25" s="18">
-        <f>E25*0.0351</f>
-        <v>702</v>
-      </c>
-      <c r="J25" s="20"/>
-      <c r="K25" s="18">
-        <f>E25*0.0724</f>
-        <v>1448.0000000000002</v>
-      </c>
-      <c r="L25" s="20"/>
-      <c r="M25" s="18">
-        <f>E25*0.1494</f>
-        <v>2988</v>
-      </c>
-      <c r="N25" s="5"/>
-    </row>
-    <row r="26" spans="2:15" ht="17.25">
-      <c r="C26" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="11">
+      <c r="E26" s="41">
         <v>143500</v>
       </c>
-      <c r="F26" s="15"/>
-      <c r="G26" s="11">
+      <c r="F26" s="25">
+        <f>E26/E$10</f>
+        <v>7.9741714641356778E-2</v>
+      </c>
+      <c r="G26" s="31">
         <f>E26*0.7432</f>
         <v>106649.2</v>
       </c>
-      <c r="H26" s="16"/>
-      <c r="I26" s="11">
+      <c r="H26" s="36"/>
+      <c r="I26" s="31">
         <f>E26*0.0351</f>
         <v>5036.8499999999995</v>
       </c>
-      <c r="J26" s="16"/>
-      <c r="K26" s="11">
+      <c r="J26" s="36"/>
+      <c r="K26" s="31">
         <f>E26*0.0724</f>
         <v>10389.400000000001</v>
       </c>
-      <c r="L26" s="16"/>
-      <c r="M26" s="11">
+      <c r="L26" s="36"/>
+      <c r="M26" s="31">
         <f>E26*0.1494-14</f>
         <v>21424.9</v>
       </c>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="2:15" ht="17.25">
+    <row r="27" spans="2:15" ht="18.75">
       <c r="C27" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="11">
+        <v>20</v>
+      </c>
+      <c r="E27" s="41">
         <v>15000</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="11">
+      <c r="F27" s="25">
+        <f>E27/E$10</f>
+        <v>8.3353708684345065E-3</v>
+      </c>
+      <c r="G27" s="31">
         <f>E27*0.7432-2</f>
         <v>11146</v>
       </c>
-      <c r="H27" s="16"/>
-      <c r="I27" s="11">
+      <c r="H27" s="36"/>
+      <c r="I27" s="31">
         <f>E27*0.0351</f>
         <v>526.5</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="11">
+      <c r="J27" s="36"/>
+      <c r="K27" s="31">
         <f>E27*0.0724</f>
         <v>1086</v>
       </c>
-      <c r="L27" s="16"/>
-      <c r="M27" s="11">
+      <c r="L27" s="36"/>
+      <c r="M27" s="31">
         <f>E27*0.1494</f>
         <v>2241</v>
       </c>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="2:15" ht="17.25">
+    <row r="28" spans="2:15" ht="18.75">
       <c r="C28" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="12">
+        <v>21</v>
+      </c>
+      <c r="E28" s="42">
         <v>2219</v>
       </c>
-      <c r="F28" s="15"/>
-      <c r="G28" s="12">
+      <c r="F28" s="26">
+        <f>E28/E$10</f>
+        <v>1.2330791971370779E-3</v>
+      </c>
+      <c r="G28" s="32">
         <f>E28*0.7432</f>
         <v>1649.1607999999999</v>
       </c>
-      <c r="H28" s="16"/>
-      <c r="I28" s="12">
+      <c r="H28" s="36"/>
+      <c r="I28" s="32">
         <f>E28*0.0351</f>
         <v>77.886899999999997</v>
       </c>
-      <c r="J28" s="16"/>
-      <c r="K28" s="12">
+      <c r="J28" s="36"/>
+      <c r="K28" s="32">
         <f>E28*0.0724</f>
         <v>160.65560000000002</v>
       </c>
-      <c r="L28" s="16"/>
-      <c r="M28" s="12">
+      <c r="L28" s="36"/>
+      <c r="M28" s="32">
         <f>E28*0.1494</f>
         <v>331.51859999999999</v>
       </c>
@@ -1364,93 +1591,95 @@
     </row>
     <row r="29" spans="2:15" ht="3" customHeight="1">
       <c r="C29" s="7"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="17"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="39"/>
       <c r="N29" s="5"/>
     </row>
     <row r="30" spans="2:15" ht="19.5">
-      <c r="C30" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="14">
+      <c r="B30" s="48"/>
+      <c r="C30" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="48"/>
+      <c r="E30" s="50">
         <f>SUM(E22:E29)</f>
-        <v>651763.19999999995</v>
-      </c>
-      <c r="F30" s="36">
+        <v>661763.19999999995</v>
+      </c>
+      <c r="F30" s="51">
         <f>E30/E10</f>
-        <v>0.3621791993598435</v>
-      </c>
-      <c r="G30" s="14">
+        <v>0.36773611327213318</v>
+      </c>
+      <c r="G30" s="52">
         <f>SUM(G22:G29)</f>
-        <v>520854.48960000003</v>
-      </c>
-      <c r="H30" s="15"/>
-      <c r="I30" s="14">
+        <v>528286.48959999997</v>
+      </c>
+      <c r="H30" s="53"/>
+      <c r="I30" s="52">
         <f>SUM(I22:I29)</f>
-        <v>27096.272799999999</v>
-      </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="14">
+        <v>27447.272799999999</v>
+      </c>
+      <c r="J30" s="53"/>
+      <c r="K30" s="52">
         <f>SUM(K22:K29)</f>
-        <v>55591.287199999999</v>
-      </c>
-      <c r="L30" s="15"/>
-      <c r="M30" s="14">
+        <v>56315.287199999999</v>
+      </c>
+      <c r="L30" s="53"/>
+      <c r="M30" s="52">
         <f>SUM(M22:M29)</f>
-        <v>48221.443200000002</v>
-      </c>
-      <c r="N30" s="5"/>
-    </row>
-    <row r="31" spans="2:15" ht="17.25">
+        <v>49715.443200000002</v>
+      </c>
+      <c r="N30" s="54"/>
+    </row>
+    <row r="31" spans="2:15" ht="18" thickBot="1">
       <c r="C31" s="7"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="17"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="13"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="2:15" ht="19.5">
-      <c r="B32" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="21">
+    <row r="32" spans="2:15" ht="20.25" thickBot="1">
+      <c r="B32" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="44">
         <f>E10-E19-E30</f>
-        <v>502315.80000000005</v>
-      </c>
-      <c r="F32" s="37">
+        <v>492315.80000000005</v>
+      </c>
+      <c r="F32" s="24">
         <f>E32/E10</f>
-        <v>0.27913256573829159</v>
-      </c>
-      <c r="G32" s="21">
+        <v>0.27357565182600196</v>
+      </c>
+      <c r="G32" s="27">
         <f>G10-G19-G30</f>
-        <v>363655.23119999998</v>
-      </c>
-      <c r="H32" s="22"/>
-      <c r="I32" s="21">
+        <v>356223.23120000004</v>
+      </c>
+      <c r="H32" s="28"/>
+      <c r="I32" s="27">
         <f>I10-I19-I30</f>
-        <v>13361.344100000009</v>
-      </c>
-      <c r="J32" s="22"/>
-      <c r="K32" s="21">
+        <v>13010.344100000009</v>
+      </c>
+      <c r="J32" s="28"/>
+      <c r="K32" s="27">
         <f>K10-K19-K30</f>
-        <v>27881.888399999989</v>
-      </c>
-      <c r="L32" s="22"/>
-      <c r="M32" s="21">
+        <v>27157.888399999989</v>
+      </c>
+      <c r="L32" s="28"/>
+      <c r="M32" s="27">
         <f>M10-M19-M30</f>
-        <v>129546.09539999999</v>
+        <v>128052.09539999999</v>
       </c>
       <c r="N32" s="5"/>
     </row>
@@ -1928,8 +2157,9 @@
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
   </mergeCells>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.15748031496062992" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>